<commit_message>
training with new filter
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\GitHub\Pig_Weight_Estimation_Pixel_Occupancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C190C002-A0FF-40C2-8AE4-6A58E628EC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D77933-1D89-42D9-90F1-416CFB574354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8CE5FD6C-ED73-4FAE-9CF9-206EAEE7ABEE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{8CE5FD6C-ED73-4FAE-9CF9-206EAEE7ABEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Model name</t>
   </si>
@@ -51,10 +51,6 @@
   </si>
   <si>
     <t>SVR</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Time Consumption</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -71,10 +67,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>LR</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>3.3s</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -83,7 +75,178 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>4.6s</t>
+    <t>Accuracy
+(For all)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Training Time</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>17.7s</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>66.3s</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>2859.4s</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>4477.8s</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Accuracy
+(For all with filtered edge)</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>Model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> Size</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0.33mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>54</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>25.9mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>26.2mb</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -91,7 +254,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +285,21 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -131,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -274,45 +452,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -322,16 +461,10 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -359,13 +492,28 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -683,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F792E1-DB5A-4340-930D-0F84AD38683E}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -694,81 +842,257 @@
     <col min="1" max="1" width="14.625" customWidth="1"/>
     <col min="2" max="2" width="23.375" customWidth="1"/>
     <col min="3" max="3" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:7" ht="19.5" thickBot="1">
+      <c r="A1" s="10"/>
+      <c r="B1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="34.5" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8">
+        <v>0.89139999999999997</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.88160000000000005</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="5" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="19.5" thickBot="1">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0.80530000000000002</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="19.5" thickBot="1"/>
+    <row r="8" spans="1:7" ht="37.5">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10">
-        <v>0.89139999999999997</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B9" s="8">
+        <v>0.86990000000000001</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>0.8508</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0.83960000000000001</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="19.5" thickBot="1">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.80010000000000003</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="19.5" thickBot="1">
+      <c r="F13">
+        <v>13.15</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="37.5">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="5" t="s">
+      <c r="D14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>12.68</v>
+      </c>
+      <c r="G14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.86990000000000001</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="F15">
+        <v>12.3</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="10">
-        <v>0.88160000000000005</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="5" t="s">
+      <c r="B16" s="8">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16">
+        <v>12.21</v>
+      </c>
+      <c r="G16">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10">
-        <v>0.84040000000000004</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="12" t="s">
+      <c r="B17" s="8">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17">
+        <v>12.17</v>
+      </c>
+      <c r="G17">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="19.5" thickBot="1">
+      <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="13">
-        <v>0.80530000000000002</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="11">
-        <v>0.78129999999999999</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>12</v>
+      <c r="B18" s="9">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <v>12.2</v>
+      </c>
+      <c r="G18">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="F19">
+        <v>12.16</v>
+      </c>
+      <c r="G19">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="F20">
+        <v>12.15</v>
+      </c>
+      <c r="G20">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="F21">
+        <v>12.14</v>
+      </c>
+      <c r="G21">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C7">
-    <sortCondition descending="1" ref="B3:B7"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C6">
+    <sortCondition descending="1" ref="B3:B6"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
update on data processing method
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niko\Documents\GitHub\Pig_Weight_Estimation_Pixel_Occupancy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D77933-1D89-42D9-90F1-416CFB574354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7508D625-A857-4B08-8208-CB91C38CDE19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="29040" xr2:uid="{8CE5FD6C-ED73-4FAE-9CF9-206EAEE7ABEE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Model name</t>
   </si>
@@ -75,11 +75,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Accuracy
-(For all)</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>Training Time</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -247,6 +242,95 @@
   </si>
   <si>
     <t>26.2mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>78.0mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>MAE</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>MSE</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>37.5mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>0.3mb</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>281.0s</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data: All data | Data entries: 38012</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>ERROR</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data: All data w/ filtering out edge | Data entries:  19755</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Accuracy</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Data: All data w/ filtering edge &amp; color range | Data entries:  9709</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -309,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -452,6 +536,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -461,7 +556,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -492,28 +587,37 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -831,10 +935,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F792E1-DB5A-4340-930D-0F84AD38683E}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22:M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -845,11 +949,11 @@
     <col min="4" max="4" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A1" s="10"/>
-      <c r="B1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="34.5" customHeight="1">
+    <row r="1" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15"/>
+    </row>
+    <row r="2" spans="1:6" ht="34.5" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,10 +961,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -871,7 +975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -882,7 +986,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -893,7 +997,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19.5" thickBot="1">
+    <row r="6" spans="1:6" ht="19.5" thickBot="1">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -904,19 +1008,25 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" thickBot="1"/>
-    <row r="8" spans="1:7" ht="37.5">
+    <row r="7" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
         <v>1</v>
       </c>
@@ -924,10 +1034,10 @@
         <v>0.86990000000000001</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
         <v>2</v>
       </c>
@@ -935,10 +1045,10 @@
         <v>0.8508</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -946,10 +1056,10 @@
         <v>0.83960000000000001</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="19.5" thickBot="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="19.5" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>3</v>
       </c>
@@ -957,145 +1067,313 @@
         <v>0.80010000000000003</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="19.5" thickBot="1">
-      <c r="F13">
-        <v>13.15</v>
-      </c>
-      <c r="G13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="37.5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="19.5" thickBot="1">
+      <c r="A13" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F14">
-        <v>12.68</v>
-      </c>
-      <c r="G14">
+      <c r="E15" s="10">
+        <v>3.72</v>
+      </c>
+      <c r="F15" s="4">
+        <v>25.33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.86990000000000001</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0.86990000000000001</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="F15">
-        <v>12.3</v>
-      </c>
-      <c r="G15">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="8">
-        <v>0.88019999999999998</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>17</v>
-      </c>
       <c r="D16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16">
-        <v>12.21</v>
-      </c>
-      <c r="G16">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>23</v>
+      </c>
+      <c r="E16" s="10">
+        <v>3.86</v>
+      </c>
+      <c r="F16" s="4">
+        <v>28.91</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="8">
         <v>0.83799999999999997</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D17" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17">
-        <v>12.17</v>
-      </c>
-      <c r="G17">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="19.5" thickBot="1">
+      <c r="E17" s="10">
+        <v>4.78</v>
+      </c>
+      <c r="F17" s="4">
+        <v>42.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="19.5" thickBot="1">
       <c r="A18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B18" s="9">
         <v>0.82399999999999995</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="E18" s="13">
+        <v>6.39</v>
+      </c>
+      <c r="F18" s="6">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="K18" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" t="s">
+        <v>24</v>
+      </c>
+      <c r="M18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="19.5" thickBot="1">
+      <c r="A19" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="J19">
+        <v>38</v>
+      </c>
+      <c r="K19">
+        <v>8.5</v>
+      </c>
+      <c r="L19">
+        <v>2.44</v>
+      </c>
+      <c r="M19">
+        <v>14.62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="37.5">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20">
+        <v>90</v>
+      </c>
+      <c r="K20">
+        <v>8.44</v>
+      </c>
+      <c r="L20">
+        <v>2.42</v>
+      </c>
+      <c r="M20">
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.90869999999999995</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="10">
+        <v>2.61</v>
+      </c>
+      <c r="F21" s="4">
+        <v>15.29</v>
+      </c>
+      <c r="J21">
+        <v>124</v>
+      </c>
+      <c r="K21">
+        <v>8.39</v>
+      </c>
+      <c r="L21">
+        <v>2.41</v>
+      </c>
+      <c r="M21">
+        <v>14.51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.91559999999999997</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="F18">
-        <v>12.2</v>
-      </c>
-      <c r="G18">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="F19">
-        <v>12.16</v>
-      </c>
-      <c r="G19">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="F20">
-        <v>12.15</v>
-      </c>
-      <c r="G20">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="F21">
-        <v>12.14</v>
-      </c>
-      <c r="G21">
-        <v>171</v>
+      <c r="E22" s="10">
+        <v>2.42</v>
+      </c>
+      <c r="F22" s="4">
+        <v>14.53</v>
+      </c>
+      <c r="J22">
+        <v>131</v>
+      </c>
+      <c r="K22">
+        <v>8.3800000000000008</v>
+      </c>
+      <c r="L22">
+        <v>2.41</v>
+      </c>
+      <c r="M22">
+        <v>14.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.8831</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="10">
+        <v>3.4</v>
+      </c>
+      <c r="F23" s="4">
+        <v>25.07</v>
+      </c>
+      <c r="J23">
+        <v>137</v>
+      </c>
+      <c r="K23">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="L23">
+        <v>2.4</v>
+      </c>
+      <c r="M23">
+        <v>14.44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="19.5" thickBot="1">
+      <c r="A24" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.89080000000000004</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="13">
+        <v>3.22</v>
+      </c>
+      <c r="F24" s="6">
+        <v>22.93</v>
+      </c>
+      <c r="J24">
+        <v>159</v>
+      </c>
+      <c r="K24">
+        <v>8.3699999999999992</v>
+      </c>
+      <c r="L24">
+        <v>2.4</v>
+      </c>
+      <c r="M24">
+        <v>14.43</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:C6">
-    <sortCondition descending="1" ref="B3:B6"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:D18">
+    <sortCondition descending="1" ref="B15:B18"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>